<commit_message>
Added initial loadout to individual archetypes
</commit_message>
<xml_diff>
--- a/CoreRulebook/Data/Archetype/Archetypes.xlsx
+++ b/CoreRulebook/Data/Archetype/Archetypes.xlsx
@@ -11,9 +11,10 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$L$8</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$J$8</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$M$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$K$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$1:$M$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$K$8</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="114">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -33,6 +34,9 @@
     <t xml:space="preserve">description</t>
   </si>
   <si>
+    <t xml:space="preserve">starting</t>
+  </si>
+  <si>
     <t xml:space="preserve">experience</t>
   </si>
   <si>
@@ -66,9 +70,16 @@
     <t xml:space="preserve">Artificer</t>
   </si>
   <si>
-    <t xml:space="preserve">{\bname{}}s are those individuals who revel in the act of creation, in making things more than the sum of their parts. 
+    <t xml:space="preserve">\bname{}s are those individuals who revel in the act of creation, in making things more than the sum of their parts. 
 Coming in many varieties – from the magic-item driven \imp{Enchanters} to the potion-mixing \imp{Alchemists} and even the more muggle-minded \imp{Technicians}, an \imp{Artificer} is both creative and technical, addressing challenges with a little something they prepared earlier. 
 Many \imp{Artificers} seal themselves away in their laboratories, only surfacing for air when absolutely necessary – but it is not unusual for some to take a more liberal approach to `field testing’ their equipment. What’s the point of creating the ultimate magical weapon if you don’t get to shoot it at things?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\spells{2}
+\spellchoice{Animate}{Forge}{Trap}{1}
+\item A choice from Potioneering Set, Runic Tools, or any mundane crafting tools.
+\orrr{The knowledge of 3 enchanting runes}{\galleon{2} of potion ingredients}{A large quantity of non-magical raw material}
+\gold{2}{1}</t>
   </si>
   <si>
     <t xml:space="preserve">\item Solve a problem using technical knowledge, innovation or one of their creations
@@ -114,15 +125,21 @@
 However\comma{} the defining trait of an \auror{} is not their combat abilities but instead their ability to discover clues\comma{} intuit motives and hunt down their foes.</t>
   </si>
   <si>
+    <t xml:space="preserve">\spells{2}
+\spellchoice{Conceal}{Halt}{Recall}{1}
+\orrr{First Aid Kit}{Navigation Tools}{Detective’s Tools}
+\item A basic weapon such as a dagger or quarterstaff
+\gold{2}{1}</t>
+  </si>
+  <si>
     <t xml:space="preserve">\item Solve a problem using investigation, tracking and detective work
 \item Track down or hunt an elusive target or solve a significant mystery</t>
   </si>
   <si>
     <t xml:space="preserve">\bonus{Insight}{\twoCape}
 \bonus{Investigation}{\twoCape}
-\bonus{Perception}{\oneCape}
-\bonus{Brawl}{\oneCape}
-\bonus{Survival}{\oneCape}</t>
+\bonus{Perception or Perception}{\twoCape}
+\bonus{Brawl}{\oneCape}</t>
   </si>
   <si>
     <t xml:space="preserve">Intuition</t>
@@ -148,9 +165,30 @@
     <t xml:space="preserve">Druid</t>
   </si>
   <si>
-    <t xml:space="preserve">A {\bname{}} is a witch or wizard who has dedicated their life to the understanding, protection and preservation of the natural order of things. 
-From the smallest fungus, to the most vicious of dragons, as well as the very bones of the Earth, and the stars in the sky – all {\bname{}}s feel a deep connection to them all. From this connection to nature, the \bname{}s draw their powers their understanding of all forms of magic is shaped into how it affects and relates to nature.
+    <t xml:space="preserve">A {\bname{}} is a witch or wizard who has dedicated their life to the understanding, protection and preservation of the natural order of things. From the smallest fungus, to the most vicious of dragons, and the very bones of the Earth, and the stars in the sky – all {\bname{}}s feel a deep connection to them all. From this connection to nature, the \bname{}s draw their powers and understanding of magic.
 In the popular mythology of \bname{}s, even in the Wizarding world, they are seen as eccentric pacifists, a pushover afraid to even hurt a fly. However, a true \bname{} understands that death and destruction are a part of the every day cycle of nature. If an old tree must burn so that a dozen new flowers may blossom, a \imp{Druid} is often more than happy to oblige. </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">\spells{1}
+\item Any two spells from the \imp{Elemental} or \imp{Bewitchment} disciplines
+\orr{First Aid Kit}{Herbology Tools}
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">\item A basic weapon such as a dagger or quarterstaff</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">\item Solve a problem by using their connection to nature
@@ -168,8 +206,7 @@
   </si>
   <si>
     <t xml:space="preserve">A \bname{} with a high innate sense of \imp{Belonging} has an intuitive, almost supernatural ability to determine when the natural, organic, order of things has been disrupted or influenced.
-By looking at a lone tree in an underground cave, such a character may attempt to discover if it \imp{Belongs} here, simply growing naturally, or if it was placed there and forced to grow by other means, or if a pack of dogs attacked out of natural instinct, or trained instructions. 
-The sense of \imp{Belonging} is not an exact art, but merely gives a \bname{} an additional insight into disruptions and alterations of nature. </t>
+By looking at a lone tree in an underground cave, such a character may attempt to discover if it \imp{Belongs} here, simply growing naturally, or if it was placed there and forced to grow by other means, or if a pack of dogs attacked out of natural instinct, or trained instructions. </t>
   </si>
   <si>
     <t xml:space="preserve">Nurture</t>
@@ -195,6 +232,12 @@
     <t xml:space="preserve">A \bname{} is a person who has dedicated themselves to the art of self-improvement, on both a spiritual level, and on a magical level. 
 \bname{}s follow the belief that before you can help others, you must first be able to help yourself. For this reason, most of their magics and abilities are focussed inwards, allowing them to improve and grow their natural abilities to supernatural levels. 
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">\spells{3}
+\spellchoice{Sustain}{Prophesy}{Seek}{1}
+\item Any choice of tool 
+\gold{1}{0}</t>
   </si>
   <si>
     <t xml:space="preserve">\item Overcome an obstacle using inner strength, or by fortifying their natural abilities
@@ -233,9 +276,40 @@
     <t xml:space="preserve">Outlaw</t>
   </si>
   <si>
-    <t xml:space="preserve">An \bname{} is someone who sits outside the normal constraints of the law (or , at Hogwarts, the rules laid down by teachers). Eternally at conflict between their own desires and those of society, many \bname{}s end up starting into a life of crime, putting their skills to more nefarious use. 
-Others turn this defiance of law and order to become perennial tricksters, revelling in chaos and uncertainty. 
+    <t xml:space="preserve">An \bname{} is someone who sits outside the normal constraints of the law (or , at Hogwarts, the rules laid down by teachers). Eternally at conflict between their own desires and those of society, many \bname{}s end up starting into a life of crime, putting their skills to more nefarious use. Others turn this defiance of law and order to become perennial tricksters, revelling in chaos and uncertainty. 
 An \bname{}, whichever path they take in life, lives and dies by their preparedness and ability to surprise those would ensnare and imprison them. Those who would catch an \bname{} should prepare to have every trick in the book thrown at them. </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">\spells{2}
+\spellchoice{Conceal}{Seek}{Bypass}{1}
+\orrr{Climbing Supplies}{Thieving Toolkit}{Tinkering Tools}
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">\item A basic weapon such as a dagger or quarterstaff
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">\gold{3}{0}</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">\item Solve a problem using trickery, deception or subterfuge
@@ -271,12 +345,65 @@
 As an adult, they are probably familiar with the workings of the penal system (and how to exploit it), whilst in Hogwarts, this knowledge can be used when questions about Detention come up. </t>
   </si>
   <si>
+    <t xml:space="preserve">Responder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A \bname{} has dedicated their life and skills towards the preservation of life, and the safety and protection of others. 
+Whilst many serve as dedicated medics in hospitals, others find themselves on the front line in the struggle against the forces of evil, patching up their allies at a crucial moment.
+Some responders recognise that preventing injuries in the first place is more effective than trying to deal with the aftermath, and so train themselves in the negation of incoming attacks. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">\spells{2}
+\spellchoice{Purify}{Resist}{Halt}{1}
+\item A \imp{First Aid Kit}, plus one other tool
+\item A light shield, bearing the symbol of the Red Cross
+\gold{2}{1}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\item Overcome a problem with care, compassion, before considering violence. 
+\item Treat a serious wound, heal an injured ally</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\bonus{Insight or Willpower}{\twoCape}
+\bonus{Kindness or Medicine}{\twoCape}
+\bonus{Medicine or Kindness}{\oneCape}
+\bonus{Willpower or Insight}{\oneCape}
+\bonus{Conviction}{\oneCape}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Triage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Things never come at you in a nice orderly queue. A \bname{} is an expert in handling multiple awful things at once, prioritising those which need immediate attention, and multitasking. 
+Whenever you must deal with multiple issues at once, when you are faced with multiple issues and need to determine which is the most pressing, or simply when most people would be overwhelmed by the problem at hand, \imp{Triage} can help you out. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steady Hand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whether it be through years of surgery training, experience holding squirming children still whilst you pry small objects from their ears, or simply your indominatable will, your hands are like rocks. 
+A \bname{} with a high \imp{Steady Hand} rating can perform delicate and precise maneouvers with their hands, without worrying about spillages, falls or mistakes. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pathology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whilst \imp{Medicine} allows you to identify and treats wounds and injuries, and identify symptoms and medical issues, the advanced knowledge of the causes of diseases, infections, disorders and even magical curses is the domain of \imp{Pathology}. 
+Though it might not help a broken ankle, a high \imp{Pathology} rating allows one to see the root cause of medical issues, and see the path needed to cure the malady. </t>
+  </si>
+  <si>
     <t xml:space="preserve">Scholar</t>
   </si>
   <si>
     <t xml:space="preserve">A \bname{} seeks to discover new knowledge, solve ancient mysteries and otherwise absorb as much information as possible, in order to further the totality of knowledge about all facets of the universe. 
 Whilst the conventional \bname{} is most at home with a chalkboard covered in symbols, or ensconced in a dusty library, most scholars these days appreciate that information, both new and old, requires stepping outside your traditional comfort zones. You can’t exactly study the behaviour of dragons without going and poking a few dragons, after all. 
 Whilst they prefer to term their adventures `field work’, there is no doubt that scholarship can sometimes be a dangerous experience. Most \bname{}s will stop at nothing, however, to help further their research. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">\spells{3}
+\item One further spell of your choice from the full spell list 
+\orr{Two non-spell books}{Any tool}
+\gold{1}{0}</t>
   </si>
   <si>
     <t xml:space="preserve">\item Use intelligence and knowledge to overcome a significant obstacle
@@ -319,6 +446,12 @@
 There are still others who are simply bluffing their way through, running the long-con and hoping nobody catches on…</t>
   </si>
   <si>
+    <t xml:space="preserve">\spells{2}
+\spellchoice{Inspire}{Delude}{Seek}{1}
+\item A fine set of clothes
+\gold{2}{3}</t>
+  </si>
+  <si>
     <t xml:space="preserve">\item Overcome a  problem using rumours, gossip or skills of persuasion and deception
 \item Turn an enemy into a friend, or otherwise significantly manipulate someone</t>
   </si>
@@ -356,6 +489,13 @@
     <t xml:space="preserve">A \bname{} is someone who is dedicated to the martial arts, trained in the use of both physical and magical combat to defeat your foes. 
 Warriors range from delicate and refined duelists, to axe-wielding maniacs. Being a warrior is more than just being handy with a weapon, however. A great warrior never goes into battle unprepared, and study and knowledge of tactics, history and the weaknesses of your foes is vital in achieving victory. 
 No matter what weapons they wield, a warrior carefully balances their combat skills, their tactical knowledge and a deep-seated rage against those who would defy them. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">\spells{2}
+\spellchoice{Infect}{Resist}{Inspire}{1}
+\item Any weapon with a proficiency requirement less than a 4-dot rating
+\item A set of medium armour
+\gold{1}{1}</t>
   </si>
   <si>
     <t xml:space="preserve">\item Overcome a problem with combat and martial prowess.
@@ -388,46 +528,6 @@
   </si>
   <si>
     <t xml:space="preserve">A \bname{} lives and dies by their knowledge of tactics. Whether it is trying to discern a viable approach to defeating a seemingly implacable foe, or recognising a strategy employed by the enemy, a \imp{Tactics} check can help reveal how an opponent functions, and what the best way to defeat them is. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Responder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A \bname{} has dedicated their life and skills towards the preservation of life, and the safety and protection of others. 
-Whilst many serve as dedicated medics in hospitals, others find themselves on the front line in the struggle against the forces of evil, patching up their allies at a crucial moment.
-Some responders recognise that preventing injuries in the first place is more effective than trying to deal with the aftermath, and so train themselves in the negation of incoming attacks. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">\item Overcome a problem with care, compassion, before considering violence. 
-\item Treat a serious wound, heal an injured ally</t>
-  </si>
-  <si>
-    <t xml:space="preserve">\bonus{Insight or Willpower}{\twoCape}
-\bonus{Kindness or Medicine}{\twoCape}
-\bonus{Medicine or Kindness}{\oneCape}
-\bonus{Willpower or Insight}{\oneCape}
-\bonus{Conviction}{\oneCape}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Triage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Things never come at you in a nice orderly queue. A \bname{} is an expert in handling multiple awful things at once, prioritising those which need immediate attention, and multitasking. 
-Whenever you must deal with multiple issues at once, when you are faced with multiple issues and need to determine which is the most pressing, or simply when most people would be overwhelmed by the problem at hand, \imp{Triage} can help you out. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Steady Hand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Whether it be through years of surgery training, experience holding squirming children still whilst you pry small objects from their ears, or simply your indominatable will, your hands are like rocks. 
-A \bname{} with a high \imp{Steady Hand} rating can perform delicate and precise maneouvers with their hands, without worrying about spillages, falls or mistakes. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pathology</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Whilst \imp{Medicine} allows you to identify and treats wounds and injuries, and identify symptoms and medical issues, the advanced knowledge of the causes of diseases, infections, disorders and even magical curses is the domain of \imp{Pathology}. 
-Though it might not help a broken ankle, a high \imp{Pathology} rating allows one to see the root cause of medical issues, and see the path needed to cure the malady. </t>
   </si>
 </sst>
 </file>
@@ -437,7 +537,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -478,6 +578,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -576,31 +681,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B7" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topRight" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="39.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="28.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="29.36"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="36.38"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="37.11"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="34.59"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="12" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="2" width="28.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="29.37"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="36.38"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="37.11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="34.59"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="13" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -613,378 +715,408 @@
       <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="5" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="7" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="145.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="144.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="J2" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="K2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" s="1" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="190.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" s="1" t="n">
+      <c r="M3" s="1" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="144.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="H4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="K4" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L4" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M4" s="1" t="n">
         <v>4</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="109.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" s="1" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="126.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" s="1" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="118.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L7" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L5" s="1" t="n">
+      <c r="M7" s="1" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L6" s="1" t="n">
+    <row r="8" customFormat="false" ht="154.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M8" s="1" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="153.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L7" s="1" t="n">
-        <v>3</v>
+    <row r="9" customFormat="false" ht="154.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M9" s="1" t="n">
+        <v>4.7</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="153.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L8" s="1" t="n">
-        <v>4.7</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="126.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L9" s="1" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="118.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="127.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>103</v>
+        <v>106</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L10" s="1" t="n">
+        <v>113</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M10" s="1" t="n">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J9"/>
+  <autoFilter ref="A1:M10"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Rejigged archetypes to look + flow better
</commit_message>
<xml_diff>
--- a/CoreRulebook/Data/Archetype/Archetypes.xlsx
+++ b/CoreRulebook/Data/Archetype/Archetypes.xlsx
@@ -11,10 +11,10 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$M$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$K$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$1:$M$8</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$K$8</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$K$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$M$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$M$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$K$8</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -138,7 +138,7 @@
   <si>
     <t xml:space="preserve">\bonus{Insight}{\twoCape}
 \bonus{Investigation}{\twoCape}
-\bonus{Perception or Perception}{\twoCape}
+\bonus{Perception or Willpower}{\twoCape}
 \bonus{Brawl}{\oneCape}</t>
   </si>
   <si>
@@ -169,26 +169,10 @@
 In the popular mythology of \bname{}s, even in the Wizarding world, they are seen as eccentric pacifists, a pushover afraid to even hurt a fly. However, a true \bname{} understands that death and destruction are a part of the every day cycle of nature. If an old tree must burn so that a dozen new flowers may blossom, a \imp{Druid} is often more than happy to oblige. </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">\spells{1}
+    <t xml:space="preserve">\spells{1}
 \item Any two spells from the \imp{Elemental} or \imp{Bewitchment} disciplines
 \orr{First Aid Kit}{Herbology Tools}
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">\item A basic weapon such as a dagger or quarterstaff</t>
-    </r>
+\item A basic weapon such as a dagger or quarterstaff</t>
   </si>
   <si>
     <t xml:space="preserve">\item Solve a problem by using their connection to nature
@@ -280,36 +264,11 @@
 An \bname{}, whichever path they take in life, lives and dies by their preparedness and ability to surprise those would ensnare and imprison them. Those who would catch an \bname{} should prepare to have every trick in the book thrown at them. </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">\spells{2}
+    <t xml:space="preserve">\spells{2}
 \spellchoice{Conceal}{Seek}{Bypass}{1}
 \orrr{Climbing Supplies}{Thieving Toolkit}{Tinkering Tools}
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">\item A basic weapon such as a dagger or quarterstaff
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">\gold{3}{0}</t>
-    </r>
+\item A basic weapon such as a dagger or quarterstaff
+\gold{3}{0}</t>
   </si>
   <si>
     <t xml:space="preserve">\item Solve a problem using trickery, deception or subterfuge
@@ -537,7 +496,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -578,11 +537,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -683,10 +637,10 @@
   </sheetPr>
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B7" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="topRight" activeCell="C11" activeCellId="0" sqref="C11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1116,7 +1070,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M10"/>
+  <autoFilter ref="A1:K9"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Completed the long-awaited ability descriptions + a few renamings
</commit_message>
<xml_diff>
--- a/CoreRulebook/Data/Archetype/Archetypes.xlsx
+++ b/CoreRulebook/Data/Archetype/Archetypes.xlsx
@@ -87,7 +87,7 @@
   </si>
   <si>
     <t xml:space="preserve">\bonus{Imbue or Craft}{\twoCape}
-\bonus{Arcane or Technology}{\twoCape}
+\bonus{Arcane or Science}{\twoCape}
 \bonus{Intelligence}{\twoCape}
 \bonus{Logic}{\oneCape}</t>
   </si>
@@ -324,8 +324,8 @@
   </si>
   <si>
     <t xml:space="preserve">\bonus{Insight or Willpower}{\twoCape}
-\bonus{Kindness or Medicine}{\twoCape}
-\bonus{Medicine or Kindness}{\oneCape}
+\bonus{Kindness or First Aid}{\twoCape}
+\bonus{First Aid or Kindness}{\oneCape}
 \bonus{Willpower or Insight}{\oneCape}
 \bonus{Conviction}{\oneCape}</t>
   </si>
@@ -347,7 +347,7 @@
     <t xml:space="preserve">Pathology</t>
   </si>
   <si>
-    <t xml:space="preserve">Whilst \imp{Medicine} allows you to identify and treats wounds and injuries, and identify symptoms and medical issues, the advanced knowledge of the causes of diseases, infections, disorders and even magical curses is the domain of \imp{Pathology}. 
+    <t xml:space="preserve">Whilst \imp{First Aid} allows you to identify and treats wounds and injuries, the advanced knowledge of the causes of diseases, infections, disorders and even magical curses is the domain of \imp{Pathology}. 
 Though it might not help a broken ankle, a high \imp{Pathology} rating allows one to see the root cause of medical issues, and see the path needed to cure the malady. </t>
   </si>
   <si>
@@ -637,10 +637,10 @@
   </sheetPr>
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="G3" activeCellId="0" sqref="G3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="D5" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topRight" activeCell="K8" activeCellId="0" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -700,7 +700,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="144.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="145.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Minor tweaks to feats
</commit_message>
<xml_diff>
--- a/CoreRulebook/Data/Archetype/Archetypes.xlsx
+++ b/CoreRulebook/Data/Archetype/Archetypes.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$K$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$M$10</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$M$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$K$9</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$M$8</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$K$8</definedName>
   </definedNames>
@@ -145,8 +145,7 @@
     <t xml:space="preserve">Intuition</t>
   </si>
   <si>
-    <t xml:space="preserve">\imp{\innateAbility} is the inherent\comma{} instinctive understanding of the minds of others possessed by an insightful and trained mind. Bypassing all \imp{Logic} and conscious reasoning\comma{} \imp{intuition} allows an \name{} to make great strides in their understanding of people and their actions by getting inside their heads and understanding the way that they think. Though not useful for solving traditional intellectual puzzles\comma{} \imp{\innateAbility} can allow an \bname{} to suddenly have a flash of insight into the motives\comma{} aims or drive of another being. 
-If you wish to know why someone would behave in a given way\comma{} why a certain shop was robbed and not another\comma{} or where a target might head next - an \name{}'s \imp{\innateAbility} is surely the best tool</t>
+    <t xml:space="preserve">\imp{\innateAbility} is the inherent\comma{} instinctive understanding of the minds of others possessed by an insightful and trained mind. Bypassing all \imp{Logic} and conscious reasoning\comma{} \imp{intuition} allows an \name{} to make great strides in their understanding of people and their actions by getting inside their heads and understanding the way that they think. \imp{\innateAbility} can allow an \bname{} to suddenly have a flash of insight into the motives\comma{} aims or drive of another being: If you wish to know why someone would behave in a given way\comma{} why a certain shop was robbed and not another\comma{} or where a target might head next - an \name{}'s \imp{\innateAbility} is surely the best tool</t>
   </si>
   <si>
     <t xml:space="preserve">Interrogate</t>
@@ -158,8 +157,7 @@
     <t xml:space="preserve">Tracking</t>
   </si>
   <si>
-    <t xml:space="preserve">Hunting down a foe is a key part of being an \bname{}, and part of that is being able to survey a scene and see where they were, what they did, and where they're going next.
-Whilst \imp{Intuition} relies on a general understanding of the target's thought pattern, when you \imp{Track} a target you look for the trail that they have left - scuffs in the dirt, broken twigs in the forest and even more abstract trails such as an online presence or a paper trail. Whatever evidence you need to find your target, \imp{Tracking} can help you out.</t>
+    <t xml:space="preserve">Hunting down a foe is a key part of being an \bname{}, and part of that is being able to survey a scene and see where they were, what they did, and where they're going next. When you \imp{Track} a target you look for the trail that they have left - scuffs in the dirt, broken twigs in the forest and even more abstract trails such as an online presence or a paper trail. </t>
   </si>
   <si>
     <t xml:space="preserve">Druid</t>
@@ -319,8 +317,8 @@
 \gold{2}{1}</t>
   </si>
   <si>
-    <t xml:space="preserve">\item Overcome a problem with care, compassion, before considering violence. 
-\item Treat a serious wound, heal an injured ally</t>
+    <t xml:space="preserve">\item Overcome a problem with care and  compassion before considering violence. 
+\item Treat a serious wound, heal an injured ally or prevent an injury from occuring </t>
   </si>
   <si>
     <t xml:space="preserve">\bonus{Insight or Willpower}{\twoCape}
@@ -473,7 +471,7 @@
   </si>
   <si>
     <t xml:space="preserve">\imp{Rage} is the deep seated anger that lies within the hearts of most people, even the most benevolent of us. A \bname{}, however, has learned to weaponise their rage, either by letting it out in an unbridled fury, or harnessing it, fuelling their cold, calculated actions. 
-Whilst in combat, \imp{Rage} can be substituted for almost any physical act, and often requires far fewer successes to achieve – attacks fuelled by rage deal an additional point of \imp{Rage}. However, on any turn on which you use \imp{Rage}, you take a 1d penalty on all resist attempts.  </t>
+Whilst in combat, \imp{Rage} can be substituted for almost any physical act such as a weapon attack, and can often serve as a useful social crutch when you need to terrify someone, or need adrenaline to lift a fallen tree from an ally. </t>
   </si>
   <si>
     <t xml:space="preserve">Command</t>
@@ -637,10 +635,10 @@
   </sheetPr>
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="D5" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-      <selection pane="topRight" activeCell="K8" activeCellId="0" sqref="K8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="C8" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topRight" activeCell="I9" activeCellId="0" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -741,7 +739,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="190.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -1070,7 +1068,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K9"/>
+  <autoFilter ref="A1:M10"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>